<commit_message>
Updated DEU_grids model - 2025-09-04 15:47
</commit_message>
<xml_diff>
--- a/VerveStacks_DEU_grids/SuppXLS/Scen_Par-AR6_R10.xlsx
+++ b/VerveStacks_DEU_grids/SuppXLS/Scen_Par-AR6_R10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_DEU_grids\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0198B8E-B374-46C2-BDE8-8D38D2D513D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C85987-4EFF-42F7-B9F9-0B07D456C121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -390,7 +390,7 @@
     <t>R10EUROPE</t>
   </si>
   <si>
-    <t xml:space="preserve"> TTF gas hub, major pellet importer </t>
+    <t>TTF gas hub, imported coal via ARA</t>
   </si>
 </sst>
 </file>

</xml_diff>